<commit_message>
Added easy live cameras streaming tests
</commit_message>
<xml_diff>
--- a/PC Server (Image Processing)/Application PC (YOLOV7)/All_IPCams.xlsx
+++ b/PC Server (Image Processing)/Application PC (YOLOV7)/All_IPCams.xlsx
@@ -8,24 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rayou\Documents\ENSTA Bretagne\MultiCam\MultiCam[Git]\PC Server (Image Processing)\Application PC (YOLOV7)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2B20C9-8B4F-49D5-9DA6-9A3B93B361DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EC1CEDD-9B5D-43DD-93E4-DCB0931A273B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E3336D2-CE27-41F0-9DA3-0D50990A723F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{8E3336D2-CE27-41F0-9DA3-0D50990A723F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IOT" sheetId="1" r:id="rId1"/>
+    <sheet name="Rayane" sheetId="2" r:id="rId2"/>
+    <sheet name="Tamara" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>cam1</t>
   </si>
@@ -42,56 +55,71 @@
     <t>CAMERA</t>
   </si>
   <si>
-    <t>IP IOT</t>
-  </si>
-  <si>
-    <t>IP TAMARA</t>
-  </si>
-  <si>
-    <t>IP RAYANE</t>
-  </si>
-  <si>
-    <t>http://172.19.147.180/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://172.19.147.182/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://172.19.147.185/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://172.19.147.186/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://192.168.43.20/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://192.168.43.137/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://192.168.43.219/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://192.168.43.220/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://192.168.43.105/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://192.168.43.144/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://192.168.43.190/cam-lo.jpg</t>
-  </si>
-  <si>
-    <t>http://192.168.43.196/cam-lo.jpg</t>
+    <t>URL IP</t>
+  </si>
+  <si>
+    <t>IOT</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>URL LOW</t>
+  </si>
+  <si>
+    <t>URL MID</t>
+  </si>
+  <si>
+    <t>URL HIGH</t>
+  </si>
+  <si>
+    <t>172.19.147.180</t>
+  </si>
+  <si>
+    <t>172.19.147.182</t>
+  </si>
+  <si>
+    <t>172.19.147.185</t>
+  </si>
+  <si>
+    <t>172.19.147.186</t>
+  </si>
+  <si>
+    <t>Rayane</t>
+  </si>
+  <si>
+    <t>Tamara</t>
+  </si>
+  <si>
+    <t>192.168.43.20</t>
+  </si>
+  <si>
+    <t>192.168.43.190</t>
+  </si>
+  <si>
+    <t>192.168.43.105</t>
+  </si>
+  <si>
+    <t>192.168.43.144</t>
+  </si>
+  <si>
+    <t>192.168.43.196</t>
+  </si>
+  <si>
+    <t>192.168.43.137</t>
+  </si>
+  <si>
+    <t>192.168.43.219</t>
+  </si>
+  <si>
+    <t>192.168.43.220</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,21 +135,263 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -129,9 +399,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -447,108 +746,495 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB819E00-7A75-4599-AE72-42785B3A9D8B}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="B1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.88671875" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" customWidth="1"/>
-    <col min="4" max="4" width="32.88671875" customWidth="1"/>
+    <col min="2" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="16"/>
+      <c r="C3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f xml:space="preserve"> HYPERLINK( _xlfn.CONCAT("http://",C4))</f>
+        <v>http://172.19.147.180</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C4,"/cam-lo.jpg"))</f>
+        <v>http://172.19.147.180/cam-lo.jpg</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK( _xlfn.CONCAT("http://",C4,"/cam-mid.jpg"))</f>
+        <v>http://172.19.147.180/cam-mid.jpg</v>
+      </c>
+      <c r="G4" s="6" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C4,"/cam-high.jpg"))</f>
+        <v>http://172.19.147.180/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f t="shared" ref="D5:D7" si="0" xml:space="preserve"> HYPERLINK( _xlfn.CONCAT("http://",C5))</f>
+        <v>http://172.19.147.182</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f t="shared" ref="E5:E7" si="1" xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C5,"/cam-lo.jpg"))</f>
+        <v>http://172.19.147.182/cam-lo.jpg</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f t="shared" ref="F5:F7" si="2" xml:space="preserve">  HYPERLINK( _xlfn.CONCAT("http://",C5,"/cam-mid.jpg"))</f>
+        <v>http://172.19.147.182/cam-mid.jpg</v>
+      </c>
+      <c r="G5" s="6" t="str">
+        <f t="shared" ref="G5:G7" si="3" xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C5,"/cam-high.jpg"))</f>
+        <v>http://172.19.147.182/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>http://172.19.147.185</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>http://172.19.147.185/cam-lo.jpg</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>http://172.19.147.185/cam-mid.jpg</v>
+      </c>
+      <c r="G6" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>http://172.19.147.185/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>http://172.19.147.186</v>
+      </c>
+      <c r="E7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>http://172.19.147.186/cam-lo.jpg</v>
+      </c>
+      <c r="F7" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>http://172.19.147.186/cam-mid.jpg</v>
+      </c>
+      <c r="G7" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>http://172.19.147.186/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H21" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F486B0D-8D79-4E6F-9002-FEA589AFFB6E}">
+  <dimension ref="B1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="16"/>
+      <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f xml:space="preserve"> HYPERLINK( _xlfn.CONCAT("http://",C4))</f>
+        <v>http://192.168.43.190</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C4,"/cam-lo.jpg"))</f>
+        <v>http://192.168.43.190/cam-lo.jpg</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK( _xlfn.CONCAT("http://",C4,"/cam-mid.jpg"))</f>
+        <v>http://192.168.43.190/cam-mid.jpg</v>
+      </c>
+      <c r="G4" s="6" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C4,"/cam-high.jpg"))</f>
+        <v>http://192.168.43.190/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f xml:space="preserve"> HYPERLINK( _xlfn.CONCAT("http://",C5))</f>
+        <v>http://192.168.43.105</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C5,"/cam-lo.jpg"))</f>
+        <v>http://192.168.43.105/cam-lo.jpg</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK( _xlfn.CONCAT("http://",C5,"/cam-mid.jpg"))</f>
+        <v>http://192.168.43.105/cam-mid.jpg</v>
+      </c>
+      <c r="G5" s="6" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C5,"/cam-high.jpg"))</f>
+        <v>http://192.168.43.105/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f xml:space="preserve"> HYPERLINK( _xlfn.CONCAT("http://",C6))</f>
+        <v>http://192.168.43.144</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C6,"/cam-lo.jpg"))</f>
+        <v>http://192.168.43.144/cam-lo.jpg</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK( _xlfn.CONCAT("http://",C6,"/cam-mid.jpg"))</f>
+        <v>http://192.168.43.144/cam-mid.jpg</v>
+      </c>
+      <c r="G6" s="6" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C6,"/cam-high.jpg"))</f>
+        <v>http://192.168.43.144/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f xml:space="preserve"> HYPERLINK( _xlfn.CONCAT("http://",C7))</f>
+        <v>http://192.168.43.196</v>
+      </c>
+      <c r="E7" s="7" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C7,"/cam-lo.jpg"))</f>
+        <v>http://192.168.43.196/cam-lo.jpg</v>
+      </c>
+      <c r="F7" s="7" t="str">
+        <f xml:space="preserve">  HYPERLINK( _xlfn.CONCAT("http://",C7,"/cam-mid.jpg"))</f>
+        <v>http://192.168.43.196/cam-mid.jpg</v>
+      </c>
+      <c r="G7" s="8" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C7,"/cam-high.jpg"))</f>
+        <v>http://192.168.43.196/cam-high.jpg</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567E5202-C9B1-4E30-B8A9-C86A7C585521}">
+  <dimension ref="B1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="16"/>
+      <c r="C3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="F3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f xml:space="preserve"> HYPERLINK( _xlfn.CONCAT("http://",C4))</f>
+        <v>http://192.168.43.20</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C4,"/cam-lo.jpg"))</f>
+        <v>http://192.168.43.20/cam-lo.jpg</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK( _xlfn.CONCAT("http://",C4,"/cam-mid.jpg"))</f>
+        <v>http://192.168.43.20/cam-mid.jpg</v>
+      </c>
+      <c r="G4" s="6" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C4,"/cam-high.jpg"))</f>
+        <v>http://192.168.43.20/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f xml:space="preserve"> HYPERLINK( _xlfn.CONCAT("http://",C5))</f>
+        <v>http://192.168.43.137</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C5,"/cam-lo.jpg"))</f>
+        <v>http://192.168.43.137/cam-lo.jpg</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK( _xlfn.CONCAT("http://",C5,"/cam-mid.jpg"))</f>
+        <v>http://192.168.43.137/cam-mid.jpg</v>
+      </c>
+      <c r="G5" s="6" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C5,"/cam-high.jpg"))</f>
+        <v>http://192.168.43.137/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f xml:space="preserve"> HYPERLINK( _xlfn.CONCAT("http://",C6))</f>
+        <v>http://192.168.43.219</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C6,"/cam-lo.jpg"))</f>
+        <v>http://192.168.43.219/cam-lo.jpg</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f xml:space="preserve">  HYPERLINK( _xlfn.CONCAT("http://",C6,"/cam-mid.jpg"))</f>
+        <v>http://192.168.43.219/cam-mid.jpg</v>
+      </c>
+      <c r="G6" s="6" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C6,"/cam-high.jpg"))</f>
+        <v>http://192.168.43.219/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D7" s="1"/>
+      <c r="C7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f xml:space="preserve"> HYPERLINK( _xlfn.CONCAT("http://",C7))</f>
+        <v>http://192.168.43.220</v>
+      </c>
+      <c r="E7" s="7" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C7,"/cam-lo.jpg"))</f>
+        <v>http://192.168.43.220/cam-lo.jpg</v>
+      </c>
+      <c r="F7" s="7" t="str">
+        <f xml:space="preserve">  HYPERLINK( _xlfn.CONCAT("http://",C7,"/cam-mid.jpg"))</f>
+        <v>http://192.168.43.220/cam-mid.jpg</v>
+      </c>
+      <c r="G7" s="8" t="str">
+        <f xml:space="preserve">  HYPERLINK(_xlfn.CONCAT("http://",C7,"/cam-high.jpg"))</f>
+        <v>http://192.168.43.220/cam-high.jpg</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="18"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{DA6FBEC0-3127-4A26-BE33-EC4A1DD93456}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{99B12765-BB78-465F-86EB-D9C02CC21752}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{6E60FBC8-4D29-4A03-AE34-5C3B315D3361}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{83E78109-FDB2-404D-A2F9-BCCC539D89B1}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{8B7981AF-7215-457E-B834-36B045A6C506}"/>
-    <hyperlink ref="D5" r:id="rId6" xr:uid="{B3297047-F5CB-4388-A847-B8BA5D2FFE10}"/>
-    <hyperlink ref="B4" r:id="rId7" xr:uid="{C517AA30-7A6B-417D-A745-85B53A14DDF7}"/>
-    <hyperlink ref="B5" r:id="rId8" xr:uid="{935221C3-2CD3-49C6-A235-F41A33BEBEFE}"/>
-    <hyperlink ref="C2" r:id="rId9" xr:uid="{A0EABEE6-0545-422D-AD92-DA5ED4E0E5E3}"/>
-    <hyperlink ref="C3" r:id="rId10" xr:uid="{3E9E8776-6138-47D2-B59D-AC29068A6999}"/>
-    <hyperlink ref="C4" r:id="rId11" xr:uid="{32233CA7-B825-47FF-B141-E24FAEBB2B21}"/>
-    <hyperlink ref="C5" r:id="rId12" xr:uid="{540F322F-9373-4DB8-B338-BA8A29C2E79F}"/>
-  </hyperlinks>
+  <mergeCells count="1">
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>